<commit_message>
chỉnh sửa quyền viết báo cáo tdg ver2
</commit_message>
<xml_diff>
--- a/backend/uploads/evidences/P1.01.01.03-Bang thong ke dien tich san xay dung HV, Giang duong - CSVC.xlsx
+++ b/backend/uploads/evidences/P1.01.01.03-Bang thong ke dien tich san xay dung HV, Giang duong - CSVC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThucTap\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7F07BE-46A2-45A3-842F-643D0F3C45F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812C2128-DCE4-4FAF-AAD8-63A70B82B943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{9C3FBDF1-1994-48D2-89B3-60325E47942D}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="template-cay-minh-chung" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="115">
   <si>
     <t>TT</t>
   </si>
@@ -31,197 +32,347 @@
     <t>Tên minh chứng</t>
   </si>
   <si>
-    <t>H2.02.01.01</t>
-  </si>
-  <si>
-    <t>Đề án thành lập của các đơn vị trực thuộc</t>
-  </si>
-  <si>
-    <t>H2.02.01.02</t>
-  </si>
-  <si>
-    <t>Quy chế tổ chức hoạt động Học viện</t>
-  </si>
-  <si>
-    <t>H2.02.01.03</t>
-  </si>
-  <si>
-    <t>Quy chế tổ chức hoạt động của các đơn vị trực thuộc</t>
-  </si>
-  <si>
-    <t>H2.02.01.04</t>
-  </si>
-  <si>
-    <t>Quy chế làm việc của ban chấp hành đảng bộ</t>
-  </si>
-  <si>
-    <t>H2.02.01.05</t>
-  </si>
-  <si>
-    <t>Nghị quyết +Chương trình/kế hoạch công tác hàng năm của Đảng ủy</t>
-  </si>
-  <si>
-    <t>H2.02.01.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quyết định thành lập HĐHV 2 nhiệm kỳ, </t>
-  </si>
-  <si>
-    <t>H2.02.01.07</t>
-  </si>
-  <si>
-    <t>Quy chế làm việc của HĐHV+ Kế hoạch, báo cáo kết quả</t>
-  </si>
-  <si>
-    <t>H2.02.01.08</t>
-  </si>
-  <si>
-    <t>Quyết định thành lập của một số HĐ như: ĐBCL, KHĐT, Lương, khen thưởng</t>
-  </si>
-  <si>
-    <t>H2.02.01.09</t>
-  </si>
-  <si>
-    <t>QĐ thành lập BCH, Quy chế hoạt động của Công đoàn, đoàn thanh niên</t>
-  </si>
-  <si>
-    <t>H2.02.01.10</t>
-  </si>
-  <si>
-    <t>Kế hoạch/chương trình giám sát của ĐU, HĐHV</t>
-  </si>
-  <si>
-    <t>H2.02.01.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Các BB họp của Đảng ủy về tổ chức quản trị </t>
-  </si>
-  <si>
-    <t>H2.02.02.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Các nghị quyết ĐU </t>
-  </si>
-  <si>
-    <t>H2.02.02.02</t>
-  </si>
-  <si>
-    <t>Quyết nghị của HĐHV, BB họp thường kỳ</t>
-  </si>
-  <si>
-    <t>H2.02.02.03</t>
-  </si>
-  <si>
-    <t>Chương trình hành động cho cả nhiệm kỳ</t>
-  </si>
-  <si>
-    <t>H2.02.02.04</t>
-  </si>
-  <si>
-    <t>Kế hoạch hành động, kế hoạch nhiệm kỳ của Ban GĐ (2016 - 2021 và 2021 - 2026)</t>
-  </si>
-  <si>
-    <t>H2.02.02.05</t>
-  </si>
-  <si>
-    <t>BB họp chỉ đao thực hiện KH</t>
-  </si>
-  <si>
-    <t>H2.02.02.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Các BB họp HĐ KH&amp;ĐT, Hội đồng tư vấn, HĐ ĐBCL</t>
-  </si>
-  <si>
-    <t>H2.02.02.07</t>
-  </si>
-  <si>
-    <t>Kế hoạch, chương trình công tác hàng năm của Công đoàn, ĐTN, HSV</t>
-  </si>
-  <si>
-    <t>H2.02.02.08</t>
-  </si>
-  <si>
-    <t>QĐ- thành lập một số Ban chỉ đạo, ban quản lý (WB, phòng chống dịch…)</t>
-  </si>
-  <si>
-    <t>H2.02.03.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QĐ phân công nhiệm vụ ĐUV theo lĩnh vực </t>
-  </si>
-  <si>
-    <t>H2.02.03.02</t>
-  </si>
-  <si>
-    <t>Báo cáo, đánh giá tổng kết các năm của ĐU</t>
-  </si>
-  <si>
-    <t>H2.02.03.03</t>
-  </si>
-  <si>
-    <t>Báo cáo tổng kết các năm của HĐHV</t>
-  </si>
-  <si>
-    <t>H2.02.03.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kế hoạch hàng năm của học viện </t>
-  </si>
-  <si>
-    <t>H2.02.03.05</t>
-  </si>
-  <si>
-    <t>BB HN CBVC hàng năm</t>
-  </si>
-  <si>
-    <t>H2.02.03.06</t>
-  </si>
-  <si>
-    <t>Các quyết định thành bổ nhiệm chức danh quản lý</t>
-  </si>
-  <si>
-    <t>H2.02.03.07</t>
-  </si>
-  <si>
-    <t>Các quyết định bổ nhiệm chức danh quản lý</t>
-  </si>
-  <si>
-    <t>H2.02.03.08</t>
-  </si>
-  <si>
-    <t>Các quyết định thành lập, thay đổi bổ sung thành viên của một số của tổ chức đoàn thể</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>Bản mô tả chương trình đào tạo</t>
-  </si>
-  <si>
-    <t>Hệ thống quản trị (bao gồm hội đồng quản trị hoặc hội đồng trường; các tổ chức đảng, đoàn thể; các hội đồng tư vấn khác) được thành lập theo quy định của pháp luật nhằm thiết lập định hướng chiến lược phù hợp với bối cảnh cụ thể của CSGD; đảm bảo trách nhiệm giải trình, tính bền vững, sự minh bạch và giảm thiểu các rủi ro tiềm tàng trong quá trình quản trị của CSGD.</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>Đề cương các học phần đầy đủ thông tin và cập nhật</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>Bản mô tả CTĐT và đề cương các học phần được công bố công khai và các bên liên quan dễ dàng tiếp cận.</t>
+    <t>H3.03.01.01</t>
+  </si>
+  <si>
+    <t>Quy chế tổ chức và hoạt động của HV, Quy định chức năng các đơn vị</t>
+  </si>
+  <si>
+    <t>H3.03.01.02</t>
+  </si>
+  <si>
+    <t>Cơ cấu tổ chức của Học viện năm 2017-2021</t>
+  </si>
+  <si>
+    <t>H3.03.01.03</t>
+  </si>
+  <si>
+    <t>Chức năng nhiệm vụ các đơn vị</t>
+  </si>
+  <si>
+    <t>H3.03.01.04</t>
+  </si>
+  <si>
+    <t>QĐ thành lập HĐ HV 2016_2021 và 2021-2026</t>
+  </si>
+  <si>
+    <t>H3.03.01.05</t>
+  </si>
+  <si>
+    <t>Quy chế tổ chức/làm việc của HĐHV_Quy chế của Đảng ủy</t>
+  </si>
+  <si>
+    <t>H3.03.01.06</t>
+  </si>
+  <si>
+    <t>Quy chế làm việc của Ban Giám đốc</t>
+  </si>
+  <si>
+    <t>H3.03.01.07</t>
+  </si>
+  <si>
+    <t>Phân công công tác của GĐ và PGĐ</t>
+  </si>
+  <si>
+    <t>H3.03.01.08</t>
+  </si>
+  <si>
+    <t>Chức năng nhiệm vụ Khoa/Viện/Trung tâm</t>
+  </si>
+  <si>
+    <t>H3.03.01.09</t>
+  </si>
+  <si>
+    <t>QĐ Ban chấp Hành đảng bộ, Công đoàn, Đoàn Thanh niên, Hội sinh viên</t>
+  </si>
+  <si>
+    <t>H3.03.01.10</t>
+  </si>
+  <si>
+    <t>H3.03.01.11</t>
+  </si>
+  <si>
+    <t>Quy chế TC và HĐ, Quy chế bổ nhiệm</t>
+  </si>
+  <si>
+    <t>H3.03.01.12</t>
+  </si>
+  <si>
+    <t>Các QĐ bổ nhiệm</t>
+  </si>
+  <si>
+    <t>H3.03.01.13</t>
+  </si>
+  <si>
+    <t>Nghị quyết Đảng ủy, HĐ Học viện, Kết luận của GĐ/PGĐ</t>
+  </si>
+  <si>
+    <t>H3.03.01.14</t>
+  </si>
+  <si>
+    <t>Quy chế làm việc của Học viện</t>
+  </si>
+  <si>
+    <t>H3.03.02.01</t>
+  </si>
+  <si>
+    <t>Quyết định Tổ công tác xây dựng chiến lược (trong đó có tầm nhìn sứ mạng</t>
+  </si>
+  <si>
+    <t>H3.03.02.02</t>
+  </si>
+  <si>
+    <t>Kế hoạch, phiếu lấy ý kiến các bên về xây dựng tầm nhìn sứ mạng</t>
+  </si>
+  <si>
+    <t>H3.03.02.03</t>
+  </si>
+  <si>
+    <t>Biên bản của Hội đồng Học viện về chiến lược</t>
+  </si>
+  <si>
+    <t>H3.03.02.04</t>
+  </si>
+  <si>
+    <t>Nghị quyết đảng ủy</t>
+  </si>
+  <si>
+    <t>H3.03.02.05</t>
+  </si>
+  <si>
+    <t>Quyết định ban hành TNSM, giá trị cốt lõi của Học viện</t>
+  </si>
+  <si>
+    <t>H3.03.02.06</t>
+  </si>
+  <si>
+    <t>Các tài liệu phát cho sinh viên, các tờ giới thiệu HV, hình ảnh chụp các pano nơi đặt tầm nhìn sứ mạng</t>
+  </si>
+  <si>
+    <t>H3.03.02.07</t>
+  </si>
+  <si>
+    <t>Kế hoạch hàng năm của Học viện</t>
+  </si>
+  <si>
+    <t>H3.03.02.08</t>
+  </si>
+  <si>
+    <t>Biên bản họp giao ban các đơn vị phổ biến quán triệt TNSM</t>
+  </si>
+  <si>
+    <t>H3.03.02.09</t>
+  </si>
+  <si>
+    <t>Nghị quyết Hội nghị đại biểu cán bộ viên chức năm học 2017-2018 đến 2021-2022</t>
+  </si>
+  <si>
+    <t>H3.03.02.10</t>
+  </si>
+  <si>
+    <t>Kế hoạch tổ chức tuần sinh hoạt công dân – HSSV các năm học 2017-2022</t>
+  </si>
+  <si>
+    <t>H3.03.02.11</t>
+  </si>
+  <si>
+    <t>Tờ rơi giới thiệu về Học viện</t>
+  </si>
+  <si>
+    <t>H3.03.02.12</t>
+  </si>
+  <si>
+    <t>H3.03.03.01</t>
+  </si>
+  <si>
+    <t>Kế hoạch kiểm tra của Ban Thanh tra/Ủy ban kiểm tra Đảng ủy năm 2017-2021</t>
+  </si>
+  <si>
+    <t>H3.03.03.02</t>
+  </si>
+  <si>
+    <t>Nghị quyết Hội nghị cán bộ viên chức năm học 2017-2018 đến 2021-2022</t>
+  </si>
+  <si>
+    <t>H3.03.03.03</t>
+  </si>
+  <si>
+    <t>Quyết định giải thể thành lập/giải thể các đơn vị giai đoạn 2017-2022</t>
+  </si>
+  <si>
+    <t>H3.03.03.04</t>
+  </si>
+  <si>
+    <t>Công văn rà soát chức năng nhiệm vụ các đơn vị chức năng</t>
+  </si>
+  <si>
+    <t>H3.03.03.05</t>
+  </si>
+  <si>
+    <t>QĐ phân công công tác của Ban Giám đốc</t>
+  </si>
+  <si>
+    <t>H3.03.03.06</t>
+  </si>
+  <si>
+    <t>Quyết định ban hành thực hiện nghị quyết số 10/NQ-CP Ban hành kèm theo Nghị quyết này Chương trình hành động của Chính phủ thực hiện Nghị quyết số 18-NQ/TW ngày 25 tháng 10 năm 2017 của Hội nghị lần thứ sáu Ban Chấp hành Trung ương Đảng khóa XII một số vấn đề về tiếp tục đổi mới, sắp xếp tổ chức bộ máy của hệ thống chính trị tinh gọn, hoạt động hiệu lực, hiệu quả; Kế hoạch số 07-KH/TW ngày 27 tháng 11 năm 2017 của Bộ Chính trị thực hiện Nghị quyết số 18-NQ/TW và Nghị quyết số 56/2017/QH14 ngày 24 tháng 11 năm 2017 của Quốc hội về việc tiếp tục cải cách tổ chức bộ máy hành chính nhà nước tinh gọn, hoạt động hiệu lực, hiệu quả</t>
+  </si>
+  <si>
+    <t>H3.03.03.07</t>
+  </si>
+  <si>
+    <t>Công văn báo cáo kết quả thực hiện nghị quyết số 18 và 19-NQ/TW</t>
+  </si>
+  <si>
+    <t>H3.03.03.08</t>
+  </si>
+  <si>
+    <t>Đề án theo NQ 19</t>
+  </si>
+  <si>
+    <t>H3.03.03.09</t>
+  </si>
+  <si>
+    <t>H3.03.03.10</t>
+  </si>
+  <si>
+    <t>H3.03.03.11</t>
+  </si>
+  <si>
+    <t>Quy chế tổ chức 2015, 2020, 2021</t>
+  </si>
+  <si>
+    <t>H3.03.03.12</t>
+  </si>
+  <si>
+    <t>Nghị định 2015 và Nghị định năm 2020</t>
+  </si>
+  <si>
+    <t>H3.03.03.13</t>
+  </si>
+  <si>
+    <t>Bản kiểm điểm của 1 số lãnh đạo, quản lý</t>
+  </si>
+  <si>
+    <t>H3.03.03.14</t>
+  </si>
+  <si>
+    <t>Biên bản họp của một số lãnh đạo quản lý</t>
+  </si>
+  <si>
+    <t>H3.03.03.15</t>
+  </si>
+  <si>
+    <t>Báo cáo tổng kết công tác lãnh đạo của Đảng bộ năm 2015 và phương hướng nhiệm vụ năm 2017 đến 2021</t>
+  </si>
+  <si>
+    <t>H3.03.03.16</t>
+  </si>
+  <si>
+    <t>Nhận xét, đánh giá của Lãnh đạo Học viện đối với Phó Giám đốc Học viện</t>
+  </si>
+  <si>
+    <t>H3.03.03.17</t>
+  </si>
+  <si>
+    <t>Kế hoạch lấy phiếu tin nhiệm giữa nhiệm kỳ</t>
+  </si>
+  <si>
+    <t>H3.03.03.18</t>
+  </si>
+  <si>
+    <t>Báo cáo kết quả đánh giá phân loại viên chức và người lao động từ 2017-2021</t>
+  </si>
+  <si>
+    <t>H3.03.03.19</t>
+  </si>
+  <si>
+    <t>Hướng dẫn đánh giá phân loại công chức, viên chức và người lao động từ 2017-2021</t>
+  </si>
+  <si>
+    <t>H3.03.03.20</t>
+  </si>
+  <si>
+    <t>Quyết định thành lập các Hội đồng: Khoa học đào tạo; Nâng lương; Học bổng; Xét tốt nghiệp; Xét điểm rèn luyện; Thi đua khen thưởng; Dừng học thôi học....</t>
+  </si>
+  <si>
+    <t>H3.03.03.21</t>
+  </si>
+  <si>
+    <t>Đề án thành lập Hội đồng Học viện 2021-2026</t>
+  </si>
+  <si>
+    <t>H3.03.03.22</t>
+  </si>
+  <si>
+    <t>Quyết định phê duyệt quy hoạch chức danh Giám đốc và Phó Giám đốc Học viện 2016-2021, 2021-2026</t>
+  </si>
+  <si>
+    <t>H3.03.03.23</t>
+  </si>
+  <si>
+    <t>Công văn chủ trương về công tác cán bộ của Học viện</t>
+  </si>
+  <si>
+    <t>H3.03.03.24</t>
+  </si>
+  <si>
+    <t>Quyết định về việc quy hoạch cán bộ quản lý các đơn vị trực thuộc Học viện: 2016-2021, 2021-2026</t>
+  </si>
+  <si>
+    <t>H3.03.03.25</t>
+  </si>
+  <si>
+    <t>Lý lịch cán bộ và nhận xét đánh giá của Nhà trường đối với cán bộ quản lý</t>
+  </si>
+  <si>
+    <t>H3.03.03.26</t>
+  </si>
+  <si>
+    <t>Công văn xây dựng vị trí việc làm</t>
+  </si>
+  <si>
+    <t>H3.03.03.27</t>
+  </si>
+  <si>
+    <t>Đề án vị trí việc làm của Học viện gửi Bộ NN và PTNT</t>
+  </si>
+  <si>
+    <t>H3.03.03.28</t>
+  </si>
+  <si>
+    <t>Quyết định phê duyệt vị trí việc làm và số người làm việc</t>
+  </si>
+  <si>
+    <t>Cấu trúc và nội dung chương trình dạy học</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>CTDH được thiết kế dựa trên CĐR.</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Đóng góp của mỗi học phần trong việc đạt được CĐR là rõ ràng.</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>CTDH có cấu trúc, trình tự logic; nội dung cập nhật và có tính tích hợp.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,18 +508,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="33">
@@ -552,7 +696,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -667,58 +811,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -764,38 +856,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1171,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E1F979-4C2E-43EA-BC33-B77BEDF24B95}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,302 +1248,539 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C34" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>56</v>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B15:C15"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>